<commit_message>
version 4: add drop down menu of sub file name
</commit_message>
<xml_diff>
--- a/mock_data.xlsx
+++ b/mock_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>身分證字號</t>
   </si>
@@ -46,15 +46,9 @@
     <t>A630702035</t>
   </si>
   <si>
-    <t>A673126970</t>
-  </si>
-  <si>
     <t>A708910406</t>
   </si>
   <si>
-    <t>A726610453</t>
-  </si>
-  <si>
     <t>A845841673</t>
   </si>
   <si>
@@ -82,13 +76,7 @@
     <t>Name_9</t>
   </si>
   <si>
-    <t>Name_17</t>
-  </si>
-  <si>
     <t>Name_14</t>
-  </si>
-  <si>
-    <t>Name_10</t>
   </si>
   <si>
     <t>Name_8</t>
@@ -449,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -476,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -484,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -492,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -500,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -508,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -516,7 +504,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -524,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -532,7 +520,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -540,23 +528,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>